<commit_message>
normalize all option & task complete GUI
</commit_message>
<xml_diff>
--- a/data/outputs/consolidated_2nd_year_1st_sem.xlsx
+++ b/data/outputs/consolidated_2nd_year_1st_sem.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -62,18 +62,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="3" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -442,20 +442,20 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="10" customWidth="1" min="1" max="1"/>
-    <col width="19" customWidth="1" min="2" max="2"/>
-    <col width="28" customWidth="1" min="3" max="3"/>
-    <col width="10" customWidth="1" min="4" max="4"/>
-    <col width="10" customWidth="1" min="5" max="5"/>
-    <col width="10" customWidth="1" min="6" max="6"/>
-    <col width="10" customWidth="1" min="7" max="7"/>
-    <col width="10" customWidth="1" min="8" max="8"/>
-    <col width="10" customWidth="1" min="9" max="9"/>
-    <col width="4" customWidth="1" min="10" max="10"/>
-    <col width="7" customWidth="1" min="11" max="11"/>
-    <col width="6" customWidth="1" min="12" max="12"/>
-    <col width="7" customWidth="1" min="13" max="13"/>
-    <col width="33" customWidth="1" min="14" max="14"/>
+    <col customWidth="1" max="1" min="1" width="10"/>
+    <col customWidth="1" max="2" min="2" width="19"/>
+    <col customWidth="1" max="3" min="3" width="28"/>
+    <col customWidth="1" max="4" min="4" width="10"/>
+    <col customWidth="1" max="5" min="5" width="10"/>
+    <col customWidth="1" max="6" min="6" width="10"/>
+    <col customWidth="1" max="7" min="7" width="10"/>
+    <col customWidth="1" max="8" min="8" width="10"/>
+    <col customWidth="1" max="9" min="9" width="10"/>
+    <col customWidth="1" max="10" min="10" width="4"/>
+    <col customWidth="1" max="11" min="11" width="7"/>
+    <col customWidth="1" max="12" min="12" width="6"/>
+    <col customWidth="1" max="13" min="13" width="7"/>
+    <col customWidth="1" max="14" min="14" width="33"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -5863,6 +5863,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>